<commit_message>
Booker API Changes test
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Datasheet.xlsx
+++ b/src/test/resources/data/Datasheet.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Data" sheetId="1" r:id="rId1"/>
     <sheet name="InValid_Data" sheetId="3" r:id="rId2"/>
     <sheet name="TESTDATA" sheetId="2" r:id="rId3"/>
+    <sheet name="ToolsQA" sheetId="4" r:id="rId4"/>
+    <sheet name="Quiter" sheetId="5" r:id="rId5"/>
+    <sheet name="SWIFT_Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>userName</t>
   </si>
@@ -51,6 +54,78 @@
   </si>
   <si>
     <t>9959@Bala</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>surName</t>
+  </si>
+  <si>
+    <t>toolsqa</t>
+  </si>
+  <si>
+    <t>quilter</t>
+  </si>
+  <si>
+    <t>chargeType</t>
+  </si>
+  <si>
+    <t>payload</t>
+  </si>
+  <si>
+    <t>ABSAZAJJXXX</t>
+  </si>
+  <si>
+    <t>BARCGB22XXX</t>
+  </si>
+  <si>
+    <t>DEBT</t>
+  </si>
+  <si>
+    <t>CRED</t>
+  </si>
+  <si>
+    <t>SHAR</t>
+  </si>
+  <si>
+    <t>BARCKENXXXX</t>
+  </si>
+  <si>
+    <t>senderBic</t>
+  </si>
+  <si>
+    <t>receiverBic</t>
+  </si>
+  <si>
+    <t>BARCZMLXXXX</t>
+  </si>
+  <si>
+    <t>BARCGHAXXXX</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;$$&lt;Document xmlns="urn:iso:std:iso:20022:tech:xsd:pacs.008.001.08"&gt;$$    &lt;FIToFICstmrCdtTrf&gt;$$        &lt;GrpHdr&gt;$$            &lt;MsgId&gt;~trno~&lt;/MsgId&gt;$$            &lt;CreDtTm&gt;~creationDate~&lt;/CreDtTm&gt; &lt;NbOfTxs&gt;1&lt;/NbOfTxs&gt;$$            &lt;TtlIntrBkSttlmAmt Ccy="~currency~"&gt;~amount~&lt;/TtlIntrBkSttlmAmt&gt;$$            &lt;IntrBkSttlmDt&gt;~valueDate~&lt;/IntrBkSttlmDt&gt;$$            &lt;SttlmInf&gt;$$                &lt;SttlmMtd&gt;CLRG&lt;/SttlmMtd&gt;$$                &lt;ClrSys&gt;$$                    &lt;Prtry&gt;SWIFT&lt;/Prtry&gt;$$                &lt;/ClrSys&gt;$$            &lt;/SttlmInf&gt;$$            &lt;InstgAgt&gt;$$                &lt;FinInstnId&gt;$$                    &lt;BICFI&gt;~senderBic~&lt;/BICFI&gt;$$                &lt;/FinInstnId&gt;$$            &lt;/InstgAgt&gt;$$            &lt;InstdAgt&gt;$$                &lt;FinInstnId&gt;$$                    &lt;BICFI&gt;~receiverBic~&lt;/BICFI&gt;$$                &lt;/FinInstnId&gt;$$            &lt;/InstdAgt&gt;$$        &lt;/GrpHdr&gt;$$        &lt;CdtTrfTxInf&gt;$$            &lt;PmtId&gt;$$                &lt;InstrId&gt;~trno~&lt;/InstrId&gt;$$                &lt;EndToEndId&gt;~trno~&lt;/EndToEndId&gt;$$                &lt;UETR&gt;~uetr~&lt;/UETR&gt; &lt;/PmtId&gt;$$            &lt;PmtTpInf&gt;$$                &lt;SvcLvl&gt;$$                    &lt;Cd&gt;G001&lt;/Cd&gt; &lt;/SvcLvl&gt;$$            &lt;/PmtTpInf&gt;$$            &lt;IntrBkSttlmAmt Ccy="~currency~"&gt;~amount~&lt;/IntrBkSttlmAmt&gt;$$            &lt;ChrgBr&gt;SLEV&lt;/ChrgBr&gt; &lt;Dbtr&gt;$$                &lt;Nm&gt;Bala Krishna&lt;/Nm&gt;$$                &lt;PstlAdr&gt;$$                    &lt;StrtNm&gt;101 Main St&lt;/StrtNm&gt;$$                    &lt;PstCd&gt;1685&lt;/PstCd&gt;$$                    &lt;TwnNm&gt;Midrand&lt;/TwnNm&gt;$$                    &lt;Ctry&gt;ZA&lt;/Ctry&gt;$$                &lt;/PstlAdr&gt;$$            &lt;/Dbtr&gt;$$            &lt;DbtrAcct&gt;$$                &lt;Id&gt;$$                    &lt;Othr&gt;$$                        &lt;Id&gt;ZA12DBTR1234567890&lt;/Id&gt;$$                    &lt;/Othr&gt;$$                &lt;/Id&gt;$$            &lt;/DbtrAcct&gt;$$            &lt;DbtrAgt&gt;$$                &lt;FinInstnId&gt;$$                    &lt;BICFI&gt;~senderBic~&lt;/BICFI&gt;$$                &lt;/FinInstnId&gt;$$            &lt;/DbtrAgt&gt;$$            &lt;CdtrAgt&gt;$$                &lt;FinInstnId&gt;$$                    &lt;BICFI&gt;~receiverBic~&lt;/BICFI&gt;$$                &lt;/FinInstnId&gt;$$            &lt;/CdtrAgt&gt;$$            &lt;Cdtr&gt;$$                &lt;Nm&gt;Bob Johnson&lt;/Nm&gt;$$                &lt;PstlAdr&gt;$$                    &lt;StrtNm&gt;202 London Rd&lt;/StrtNm&gt;$$                    &lt;PstCd&gt;SW1A 0AA&lt;/PstCd&gt;$$                    &lt;TwnNm&gt;London&lt;/TwnNm&gt;$$                    &lt;Ctry&gt;GB&lt;/Ctry&gt;$$                &lt;/PstlAdr&gt;$$            &lt;/Cdtr&gt;$$            &lt;CdtrAcct&gt;$$                &lt;Id&gt;$$                    &lt;IBAN&gt;GB98BANK12345678901234&lt;/IBAN&gt;$$                &lt;/Id&gt;$$            &lt;/CdtrAcct&gt;$$            &lt;RmtInf&gt;$$                &lt;Ustrd&gt;Payment for services rendered&lt;/Ustrd&gt;$$            &lt;/RmtInf&gt;$$        &lt;/CdtTrfTxInf&gt;$$    &lt;/FIToFICstmrCdtTrf&gt;$$&lt;/Document&gt;</t>
   </si>
 </sst>
 </file>
@@ -117,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,12 +215,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -155,6 +241,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,7 +582,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -518,7 +622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -556,4 +662,200 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="4" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="9" customFormat="1">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="9" customFormat="1">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="9" customFormat="1">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="9" customFormat="1">
+      <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>